<commit_message>
Purchase / Order Register
</commit_message>
<xml_diff>
--- a/RDLC Reports Format/Nov-21/Purchase Order Register/Purchase Order Register format.xlsx
+++ b/RDLC Reports Format/Nov-21/Purchase Order Register/Purchase Order Register format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive E\bipro\tally report format\Purchase Order register\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\GIT\MendinePharmaceuticalsPvtLtd\Mendine_TallyReportPortal\RDLC Reports Format\Nov-21\Purchase Order Register\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D87462B-D26F-487D-B255-C3C9B6E953AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72736AB3-7E1E-40E1-9948-A4BE20E68CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,10 +497,10 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;&quot;0&quot; Pcs&quot;"/>
-    <numFmt numFmtId="167" formatCode="&quot;&quot;0.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;&quot;0&quot; Strip&quot;"/>
-    <numFmt numFmtId="169" formatCode="&quot;&quot;0.0000&quot; Kgs&quot;"/>
-    <numFmt numFmtId="170" formatCode="&quot;&quot;0.0000&quot; Ltr.&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;&quot;0.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;&quot;0&quot; Strip&quot;"/>
+    <numFmt numFmtId="168" formatCode="&quot;&quot;0.0000&quot; Kgs&quot;"/>
+    <numFmt numFmtId="169" formatCode="&quot;&quot;0.0000&quot; Ltr.&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -610,7 +610,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -619,16 +619,16 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -913,26 +913,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44203</v>
       </c>
@@ -999,7 +999,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>44203</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>44203</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>44203</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>44203</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>44204</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>44204</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>44212</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>44212</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>44212</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>44212</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>44217</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>44155</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>44217</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>44217</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>44217</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>44217</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>44217</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>44217</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>44218</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>44218</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>44220</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>44220</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>44220</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>44220</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>44220</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>44220</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>44220</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>44220</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>44223</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>44223</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>44223</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>44223</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>44225</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>44225</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>44225</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>44225</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>44226</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>44226</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>44226</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>44226</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>44198</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>44198</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>44198</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>44198</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>44199</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>44199</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>44199</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>44199</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>44200</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>44200</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>44200</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>44200</v>
       </c>
@@ -1888,7 +1888,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>44200</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>44200</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>44201</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>44201</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>44201</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>44201</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>44203</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44203</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>44203</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>44203</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>43840</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>44204</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>44221</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>44207</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>44207</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>44214</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>44207</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>44216</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>44211</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>44226</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>44211</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>44211</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>44211</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>44211</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>44211</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>44212</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>44212</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>44212</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>44212</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>44214</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>44214</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>44215</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>44215</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>44215</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>44216</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>44226</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>44218</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>44218</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>44218</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>44218</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>44218</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>44218</v>
       </c>
@@ -2624,7 +2624,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>44218</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>44218</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>44218</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>44218</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>44220</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>44220</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>44223</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>44223</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>44223</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>44223</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>44224</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>44232</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>44224</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>44232</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>44224</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>44232</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>44225</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>44225</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>44225</v>
       </c>

</xml_diff>